<commit_message>
Day 5, MD5 post complete
</commit_message>
<xml_diff>
--- a/aoc/d5runtimes.xlsx
+++ b/aoc/d5runtimes.xlsx
@@ -13,13 +13,13 @@
   </sheets>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Algorithm</t>
   </si>
@@ -130,24 +130,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.000"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -263,7 +248,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A15:F18" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -341,7 +326,7 @@
     <dataField name="Average of Gen2" fld="5" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -644,7 +629,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A24" sqref="A24:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,6 +867,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>

</xml_diff>